<commit_message>
HEEDLS-891 Add PRN to delegate upload journey
</commit_message>
<xml_diff>
--- a/DigitalLearningSolutions.Data.Tests/TestData/DelegateUploadTest.xlsx
+++ b/DigitalLearningSolutions.Data.Tests/TestData/DelegateUploadTest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alejac\Git\DLSV2\DigitalLearningSolutions.Data.Tests\Services\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alejac\Git\DLSV2\DigitalLearningSolutions.Data.Tests\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BDD2C27-E052-48DA-8B0D-81993A7E1B7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660D4309-65A4-442F-8D11-70D0B47F2E1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23136" yWindow="-96" windowWidth="23232" windowHeight="13992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DelegatesBulkUpload" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>LastName</t>
   </si>
@@ -111,6 +111,15 @@
   </si>
   <si>
     <t>Health Professional</t>
+  </si>
+  <si>
+    <t>HasPRN</t>
+  </si>
+  <si>
+    <t>PRN</t>
+  </si>
+  <si>
+    <t>MammalHands</t>
   </si>
 </sst>
 </file>
@@ -153,9 +162,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -175,9 +185,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:M4" totalsRowShown="0">
-  <autoFilter ref="A1:M4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:O4" totalsRowShown="0">
+  <autoFilter ref="A1:O4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="LastName"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="FirstName"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="DelegateID"/>
@@ -191,6 +201,8 @@
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Answer6"/>
     <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Active"/>
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="EmailAddress"/>
+    <tableColumn id="14" xr3:uid="{FA40E1EF-5652-4F78-928E-56D1B26E86E0}" name="HasPRN"/>
+    <tableColumn id="15" xr3:uid="{413752CE-C2EC-47CB-9194-82364E4E4C03}" name="PRN"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -492,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,9 +522,11 @@
     <col min="8" max="11" width="12" customWidth="1"/>
     <col min="12" max="12" width="9.85546875" customWidth="1"/>
     <col min="13" max="13" width="24.42578125" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -552,8 +566,14 @@
       <c r="M1" t="s">
         <v>12</v>
       </c>
+      <c r="N1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -572,8 +592,12 @@
       <c r="M2" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="N2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O2" s="2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -595,8 +619,10 @@
       <c r="L3" t="b">
         <v>1</v>
       </c>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -617,6 +643,12 @@
       </c>
       <c r="L4" t="b">
         <v>1</v>
+      </c>
+      <c r="N4" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>